<commit_message>
added options and question modes
</commit_message>
<xml_diff>
--- a/quiz questions.xlsx
+++ b/quiz questions.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\quizbuilder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B366CED-0CF2-4C23-814D-1F2AAD9BFD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA68C81-5A08-411D-92E4-E2F9C201AEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="0" windowWidth="17200" windowHeight="10500" xr2:uid="{668E23A6-9E5B-4CA6-B803-DF2886CE1CEA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="questions" sheetId="1" r:id="rId1"/>
+    <sheet name="options" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Question</t>
   </si>
@@ -102,18 +103,12 @@
     <t>Correctanswer</t>
   </si>
   <si>
-    <t>Who is the best?</t>
-  </si>
-  <si>
     <t>What is their quest?</t>
   </si>
   <si>
     <t>To make quizes work</t>
   </si>
   <si>
-    <t>What is your favourite colour</t>
-  </si>
-  <si>
     <t>yellow</t>
   </si>
   <si>
@@ -126,20 +121,50 @@
     <t>red</t>
   </si>
   <si>
-    <t>What is the capital of Assyria</t>
-  </si>
-  <si>
     <t>Assur</t>
   </si>
   <si>
     <t>Asur</t>
+  </si>
+  <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t>Randomised</t>
+  </si>
+  <si>
+    <t>Scored</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>click the correct answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5+2 = </t>
+  </si>
+  <si>
+    <t>What is your name?</t>
+  </si>
+  <si>
+    <t>What is your favourite colour?</t>
+  </si>
+  <si>
+    <t>What is the capital of Assyria?</t>
+  </si>
+  <si>
+    <t>&amp;lt;&amp;LT;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +177,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF333322"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -174,11 +205,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,7 +528,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -531,10 +563,13 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -554,14 +589,16 @@
       <c r="G2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
@@ -574,43 +611,49 @@
       <c r="G3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -632,20 +675,32 @@
       <c r="G6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="1">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1">
+        <v>9</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
+      <c r="A8" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -655,7 +710,7 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
+      <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -677,5 +732,48 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2EDAB20-1AEA-4826-9EC9-1A40AFE2F38B}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
math jax working loop mode working
</commit_message>
<xml_diff>
--- a/quiz questions.xlsx
+++ b/quiz questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\quizbuilder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34459A5-2AA5-45D3-9C2E-491C73565C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EF5FE0-3121-49EE-A3DD-8946CDA0ED72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{668E23A6-9E5B-4CA6-B803-DF2886CE1CEA}"/>
+    <workbookView xWindow="20" yWindow="30" windowWidth="17560" windowHeight="9840" xr2:uid="{668E23A6-9E5B-4CA6-B803-DF2886CE1CEA}"/>
   </bookViews>
   <sheets>
     <sheet name="questions" sheetId="1" r:id="rId1"/>
@@ -157,13 +157,13 @@
     <t>loopincorrect</t>
   </si>
   <si>
-    <t>$x^2 + x^3$</t>
-  </si>
-  <si>
-    <t>$x^2 * x^3$</t>
-  </si>
-  <si>
-    <t>$x^5$</t>
+    <t>${x^2 * x^3}$</t>
+  </si>
+  <si>
+    <t>${x^5}$</t>
+  </si>
+  <si>
+    <t>${x^2 + x^3}$</t>
   </si>
 </sst>
 </file>
@@ -541,7 +541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5135FCE6-9BDC-4580-82A2-9614BC0DD28A}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -695,13 +695,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>

</xml_diff>

<commit_message>
some other ideas, issues with tabs!
</commit_message>
<xml_diff>
--- a/quiz questions.xlsx
+++ b/quiz questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\quizbuilder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EF5FE0-3121-49EE-A3DD-8946CDA0ED72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A930BC90-C977-4FA1-8B4A-31D83A348A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="30" windowWidth="17560" windowHeight="9840" xr2:uid="{668E23A6-9E5B-4CA6-B803-DF2886CE1CEA}"/>
+    <workbookView xWindow="950" yWindow="660" windowWidth="17560" windowHeight="9840" xr2:uid="{668E23A6-9E5B-4CA6-B803-DF2886CE1CEA}"/>
   </bookViews>
   <sheets>
     <sheet name="questions" sheetId="1" r:id="rId1"/>
@@ -157,13 +157,13 @@
     <t>loopincorrect</t>
   </si>
   <si>
+    <t>${x^5}$</t>
+  </si>
+  <si>
+    <t>${x^2 + x^3}$</t>
+  </si>
+  <si>
     <t>${x^2 * x^3}$</t>
-  </si>
-  <si>
-    <t>${x^5}$</t>
-  </si>
-  <si>
-    <t>${x^2 + x^3}$</t>
   </si>
 </sst>
 </file>
@@ -542,7 +542,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -695,13 +695,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>

</xml_diff>